<commit_message>
time to start testing. fun fun.
</commit_message>
<xml_diff>
--- a/OS/a4/results.xlsx
+++ b/OS/a4/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,11 +59,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,11 +83,19 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -222,7 +231,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -258,7 +267,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Deadlock (%) vs Queue Size (5 Consumer)</a:t>
+              <a:t>Deadlock (%) vs Queue Size (200 Donuts)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -305,6 +314,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -319,28 +329,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>26600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>26700</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>26800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>27500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>28000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>28500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -352,19 +362,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -380,15 +390,15 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="3474361"/>
-        <c:axId val="80970207"/>
+        <c:axId val="40856962"/>
+        <c:axId val="32563971"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3474361"/>
+        <c:axId val="40856962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="80"/>
-          <c:min val="10"/>
+          <c:max val="28500"/>
+          <c:min val="26500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -439,7 +449,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -468,12 +478,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80970207"/>
+        <c:crossAx val="32563971"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80970207"/>
+        <c:axId val="32563971"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +536,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -555,7 +565,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3474361"/>
+        <c:crossAx val="40856962"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -582,7 +592,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -618,7 +628,8 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Consumer Count vs Avg Deadlock (%)</a:t>
+              <a:t>Dozens of Donuts
+ vs Avg Deadlock (%)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -665,6 +676,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -679,34 +691,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,46 +733,46 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1538465"/>
-        <c:axId val="8373043"/>
+        <c:axId val="45395847"/>
+        <c:axId val="60254096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1538465"/>
+        <c:axId val="45395847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
-          <c:min val="1"/>
+          <c:max val="300"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -795,14 +807,14 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Number of Consumers</a:t>
+                  <a:t>Dozens of Donuts</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -831,14 +843,15 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8373043"/>
+        <c:crossAx val="60254096"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8373043"/>
+        <c:axId val="60254096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -889,7 +902,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -918,8 +931,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538465"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="45395847"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -950,15 +963,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>335880</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>711720</xdr:colOff>
+      <xdr:colOff>1047240</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -966,8 +979,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="1778400"/>
-        <a:ext cx="5759640" cy="3241800"/>
+        <a:off x="335880" y="1740240"/>
+        <a:ext cx="5692680" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -980,15 +993,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:colOff>385200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>711720</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:colOff>1096560</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -996,8 +1009,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="7242480"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="385200" y="6859800"/>
+        <a:ext cx="5692680" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1015,20 +1028,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E43"/>
+  <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,17 +1063,11 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>5</v>
+        <v>26500</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">((B3+C3)/2)*20</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
@@ -1068,73 +1075,43 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>5</v>
+        <v>26600</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">((B4+C4)/2)*20</f>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>4</v>
+        <v>26700</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">((B5+C5)/2)*20</f>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>26800</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">((B6+C6)/2)*20</f>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">((B7+C7)/2)*20</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0</v>
+        <v>27500</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">((B8+C8)/2)*20</f>
@@ -1143,13 +1120,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">((B9+C9)/2)*20</f>
@@ -1158,13 +1129,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0</v>
+        <v>28500</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">((B10+C10)/2)*20</f>
@@ -1172,28 +1137,22 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D34" s="3" t="n">
         <f aca="false">((B34+C34)/2)*20</f>
@@ -1202,137 +1161,56 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D35" s="3" t="n">
         <f aca="false">((B35+C35)/2)*20</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="D36" s="3" t="n">
         <f aca="false">((B36+C36)/2)*20</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D37" s="3" t="n">
         <f aca="false">((B37+C37)/2)*20</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="D38" s="3" t="n">
         <f aca="false">((B38+C38)/2)*20</f>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="D39" s="3" t="n">
         <f aca="false">((B39+C39)/2)*20</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>4</v>
+        <v>300</v>
       </c>
       <c r="D40" s="3" t="n">
         <f aca="false">((B40+C40)/2)*20</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D41" s="3" t="n">
-        <f aca="false">((B41+C41)/2)*20</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="n">
-        <f aca="false">((B42+C42)/2)*20</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D43" s="3" t="n">
-        <f aca="false">((B43+C43)/2)*20</f>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
process halt whatever seems to work, time to test AGAIN.
</commit_message>
<xml_diff>
--- a/OS/a4/results.xlsx
+++ b/OS/a4/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">Queue Size</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">4 cores / 8 threads</t>
   </si>
   <si>
+    <t xml:space="preserve">200 donuts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consumers</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% Queue Size</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -332,25 +338,25 @@
                   <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26600</c:v>
+                  <c:v>26700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26700</c:v>
+                  <c:v>26800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26800</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27000</c:v>
+                  <c:v>27500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27500</c:v>
+                  <c:v>28000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28000</c:v>
+                  <c:v>28500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28500</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,13 +368,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -390,11 +396,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40856962"/>
-        <c:axId val="32563971"/>
+        <c:axId val="10364695"/>
+        <c:axId val="52320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40856962"/>
+        <c:axId val="10364695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28500"/>
@@ -478,14 +484,16 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32563971"/>
+        <c:crossAx val="52320"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32563971"/>
+        <c:axId val="52320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -565,8 +573,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40856962"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="10364695"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -592,7 +600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -764,11 +772,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45395847"/>
-        <c:axId val="60254096"/>
+        <c:axId val="68020671"/>
+        <c:axId val="90731107"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45395847"/>
+        <c:axId val="68020671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -843,15 +851,16 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60254096"/>
+        <c:crossAx val="90731107"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60254096"/>
+        <c:axId val="90731107"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -931,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45395847"/>
+        <c:crossAx val="68020671"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1030,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1065,9 +1074,15 @@
       <c r="A3" s="0" t="n">
         <v>26500</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="D3" s="0" t="n">
         <f aca="false">((B3+C3)/2)*20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
@@ -1075,25 +1090,40 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>26600</v>
+        <v>26700</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">((B4+C4)/2)*20</f>
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>26700</v>
+        <v>26800</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">((B5+C5)/2)*20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>26800</v>
+        <v>27000</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">((B6+C6)/2)*20</f>
@@ -1102,7 +1132,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>27000</v>
+        <v>27500</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">((B7+C7)/2)*20</f>
@@ -1111,7 +1141,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>27500</v>
+        <v>28000</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">((B8+C8)/2)*20</f>
@@ -1120,7 +1150,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>28000</v>
+        <v>28500</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">((B9+C9)/2)*20</f>
@@ -1128,9 +1158,6 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>28500</v>
-      </c>
       <c r="D10" s="0" t="n">
         <f aca="false">((B10+C10)/2)*20</f>
         <v>0</v>
@@ -1138,16 +1165,19 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,6 +1188,9 @@
         <f aca="false">((B34+C34)/2)*20</f>
         <v>0</v>
       </c>
+      <c r="E34" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1166,6 +1199,9 @@
       <c r="D35" s="3" t="n">
         <f aca="false">((B35+C35)/2)*20</f>
         <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
results are in, now to writeup.
</commit_message>
<xml_diff>
--- a/OS/a4/results.xlsx
+++ b/OS/a4/results.xlsx
@@ -237,7 +237,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -371,19 +371,19 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -396,11 +396,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="10364695"/>
-        <c:axId val="52320"/>
+        <c:axId val="51817671"/>
+        <c:axId val="40860163"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10364695"/>
+        <c:axId val="51817671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28500"/>
@@ -484,12 +484,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52320"/>
+        <c:crossAx val="40860163"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52320"/>
+        <c:axId val="40860163"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -573,7 +573,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10364695"/>
+        <c:crossAx val="51817671"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,7 +600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -744,19 +744,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -772,11 +772,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="68020671"/>
-        <c:axId val="90731107"/>
+        <c:axId val="33268449"/>
+        <c:axId val="13395770"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68020671"/>
+        <c:axId val="33268449"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -851,12 +851,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90731107"/>
+        <c:crossAx val="13395770"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90731107"/>
+        <c:axId val="13395770"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -940,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68020671"/>
+        <c:crossAx val="33268449"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1093,14 +1093,14 @@
         <v>26700</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">((B4+C4)/2)*20</f>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -1111,46 +1111,70 @@
         <v>26800</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">((B5+C5)/2)*20</f>
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>27000</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="D6" s="0" t="n">
         <f aca="false">((B6+C6)/2)*20</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>27500</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="D7" s="0" t="n">
         <f aca="false">((B7+C7)/2)*20</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>28000</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D8" s="0" t="n">
         <f aca="false">((B8+C8)/2)*20</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>28500</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">((B9+C9)/2)*20</f>
@@ -1184,6 +1208,12 @@
       <c r="A34" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D34" s="3" t="n">
         <f aca="false">((B34+C34)/2)*20</f>
         <v>0</v>
@@ -1196,6 +1226,12 @@
       <c r="A35" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D35" s="3" t="n">
         <f aca="false">((B35+C35)/2)*20</f>
         <v>0</v>
@@ -1208,45 +1244,75 @@
       <c r="A36" s="0" t="n">
         <v>175</v>
       </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="D36" s="3" t="n">
         <f aca="false">((B36+C36)/2)*20</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="B37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="D37" s="3" t="n">
         <f aca="false">((B37+C37)/2)*20</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>225</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="D38" s="3" t="n">
         <f aca="false">((B38+C38)/2)*20</f>
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>250</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="D39" s="3" t="n">
         <f aca="false">((B39+C39)/2)*20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>300</v>
       </c>
+      <c r="B40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="D40" s="3" t="n">
         <f aca="false">((B40+C40)/2)*20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
will copy over and see if it works
</commit_message>
<xml_diff>
--- a/OS/a4/results.xlsx
+++ b/OS/a4/results.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">200 donuts</t>
   </si>
   <si>
-    <t xml:space="preserve">Consumers</t>
+    <t xml:space="preserve">Dozens of Donuts</t>
   </si>
   <si>
     <t xml:space="preserve">Trial 1</t>
@@ -237,7 +237,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -396,11 +396,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51817671"/>
-        <c:axId val="40860163"/>
+        <c:axId val="64678440"/>
+        <c:axId val="71284969"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51817671"/>
+        <c:axId val="64678440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28500"/>
@@ -484,12 +484,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40860163"/>
+        <c:crossAx val="71284969"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40860163"/>
+        <c:axId val="71284969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -573,7 +573,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51817671"/>
+        <c:crossAx val="64678440"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,7 +600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -772,11 +772,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33268449"/>
-        <c:axId val="13395770"/>
+        <c:axId val="12921694"/>
+        <c:axId val="3374227"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33268449"/>
+        <c:axId val="12921694"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -851,12 +851,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13395770"/>
+        <c:crossAx val="3374227"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13395770"/>
+        <c:axId val="3374227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -940,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33268449"/>
+        <c:crossAx val="12921694"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
adding results. updated README.
</commit_message>
<xml_diff>
--- a/OS/a4/results.xlsx
+++ b/OS/a4/results.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -237,7 +237,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -290,7 +290,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$D$2</c:f>
+              <c:f>Results!$D$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -330,7 +330,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:f>Results!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -363,7 +363,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$10</c:f>
+              <c:f>Results!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -371,16 +371,16 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
@@ -396,11 +396,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="64678440"/>
-        <c:axId val="71284969"/>
+        <c:axId val="52897045"/>
+        <c:axId val="29083137"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64678440"/>
+        <c:axId val="52897045"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28500"/>
@@ -484,12 +484,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71284969"/>
+        <c:crossAx val="29083137"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71284969"/>
+        <c:axId val="29083137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -573,7 +573,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64678440"/>
+        <c:crossAx val="52897045"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,7 +600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -654,7 +654,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$33:$D$33</c:f>
+              <c:f>Results!$D$33:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -694,7 +694,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$43</c:f>
+              <c:f>Results!$A$34:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -733,7 +733,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$34:$D$43</c:f>
+              <c:f>Results!$D$34:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -772,11 +772,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="12921694"/>
-        <c:axId val="3374227"/>
+        <c:axId val="467782"/>
+        <c:axId val="81585602"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12921694"/>
+        <c:axId val="467782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -851,12 +851,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3374227"/>
+        <c:crossAx val="81585602"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3374227"/>
+        <c:axId val="81585602"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -940,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12921694"/>
+        <c:crossAx val="467782"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1093,14 +1093,14 @@
         <v>26700</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">((B4+C4)/2)*20</f>
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -1111,14 +1111,14 @@
         <v>26800</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">((B5+C5)/2)*20</f>
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,14 +1126,14 @@
         <v>27000</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">((B6+C6)/2)*20</f>
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,11 +1144,11 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">((B7+C7)/2)*20</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>